<commit_message>
[Drop]: DefaultProjectManagement + UserNotificationManagement FR
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/DefaultProjectManagement/DefaultProjectManagement Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/DefaultProjectManagement/DefaultProjectManagement Specification.xlsx
@@ -54,7 +54,7 @@
     <t xml:space="preserve">  - Người dùng chọn More Action của Menu.
 - Hệ thống hiển thị sidebar.
 - Người dùng chọn Manage Default Project.
-- Hệ thống hiển thị danh mục các tùy chọn mặc định.
+- Hệ thống hiển thị danh mục các Dự án mặc định.
 - Người dùng lựa chọn một trong các Dự án mặc định để truy cập.
 - Hệ thống lấy dữ liệu tương ứng từ CSDL và Hiển thị.</t>
   </si>
@@ -263,10 +263,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -295,13 +295,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -315,15 +308,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,6 +331,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -345,25 +377,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -376,17 +402,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -398,52 +431,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -454,187 +454,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,15 +685,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -752,6 +743,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -769,168 +780,157 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1213,8 +1213,8 @@
   <sheetPr/>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="13.2" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
[Add]: DefaultProjectManagement + UserNotificationManagement Specification Tổng quát
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/DefaultProjectManagement/DefaultProjectManagement Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/DefaultProjectManagement/DefaultProjectManagement Specification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9204"/>
+    <workbookView windowWidth="23040" windowHeight="9204" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Manage Default Project" sheetId="14" r:id="rId1"/>
@@ -19,9 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="60">
   <si>
     <t>Use-case number:</t>
+  </si>
+  <si>
+    <t>UC9</t>
   </si>
   <si>
     <t>Use-case name:</t>
@@ -263,10 +266,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -294,6 +297,51 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -301,10 +349,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -317,53 +381,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -377,6 +395,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -386,23 +412,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,27 +441,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -454,187 +457,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,26 +692,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -729,16 +741,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -762,42 +789,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -807,130 +810,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1213,8 +1216,8 @@
   <sheetPr/>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="13.2" outlineLevelCol="2"/>
@@ -1226,109 +1229,111 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" ht="50" customHeight="1" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" ht="50" customHeight="1" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" ht="50" customHeight="1" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="50" customHeight="1" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" ht="197" customHeight="1" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" ht="50" customHeight="1" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" ht="50" customHeight="1" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" ht="50" customHeight="1" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" ht="50" customHeight="1" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" ht="50" customHeight="1" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" ht="50" customHeight="1" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -1355,8 +1360,8 @@
   <sheetPr/>
   <dimension ref="C2:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="13.2" outlineLevelCol="4"/>
@@ -1368,109 +1373,111 @@
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" ht="50" customHeight="1" spans="3:5">
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" ht="50" customHeight="1" spans="3:5">
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" ht="50" customHeight="1" spans="3:5">
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" ht="50" customHeight="1" spans="3:5">
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" ht="200" customHeight="1" spans="3:5">
       <c r="C7" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" ht="50" customHeight="1" spans="3:5">
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" ht="50" customHeight="1" spans="3:5">
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" ht="50" customHeight="1" spans="3:5">
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" ht="50" customHeight="1" spans="3:5">
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" ht="50" customHeight="1" spans="3:5">
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" ht="50" customHeight="1" spans="3:5">
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5"/>
     </row>
@@ -1497,8 +1504,8 @@
   <sheetPr/>
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="13.2" outlineLevelCol="4"/>
@@ -1510,109 +1517,111 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="50" customHeight="1" spans="3:5">
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" ht="50" customHeight="1" spans="3:5">
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" ht="50" customHeight="1" spans="3:5">
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" ht="50" customHeight="1" spans="3:5">
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="199" customHeight="1" spans="3:5">
       <c r="C8" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" ht="50" customHeight="1" spans="3:5">
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" ht="50" customHeight="1" spans="3:5">
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" ht="50" customHeight="1" spans="3:5">
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" ht="50" customHeight="1" spans="3:5">
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" ht="50" customHeight="1" spans="3:5">
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" ht="50" customHeight="1" spans="3:5">
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1639,8 +1648,8 @@
   <sheetPr/>
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="13.2" outlineLevelCol="4"/>
@@ -1652,109 +1661,111 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="50" customHeight="1" spans="3:5">
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" ht="50" customHeight="1" spans="3:5">
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" ht="50" customHeight="1" spans="3:5">
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" ht="50" customHeight="1" spans="3:5">
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="199" customHeight="1" spans="3:5">
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" ht="50" customHeight="1" spans="3:5">
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" ht="50" customHeight="1" spans="3:5">
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" ht="50" customHeight="1" spans="3:5">
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" ht="50" customHeight="1" spans="3:5">
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" ht="50" customHeight="1" spans="3:5">
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" ht="50" customHeight="1" spans="3:5">
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1781,8 +1792,8 @@
   <sheetPr/>
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="13.2" outlineLevelCol="4"/>
@@ -1794,109 +1805,111 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="50" customHeight="1" spans="3:5">
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" ht="50" customHeight="1" spans="3:5">
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" ht="50" customHeight="1" spans="3:5">
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" ht="50" customHeight="1" spans="3:5">
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="198" customHeight="1" spans="3:5">
       <c r="C8" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" ht="50" customHeight="1" spans="3:5">
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" ht="50" customHeight="1" spans="3:5">
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" ht="50" customHeight="1" spans="3:5">
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" ht="50" customHeight="1" spans="3:5">
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" ht="50" customHeight="1" spans="3:5">
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" ht="50" customHeight="1" spans="3:5">
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1923,8 +1936,8 @@
   <sheetPr/>
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="13.2" outlineLevelCol="4"/>
@@ -1936,109 +1949,111 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="50" customHeight="1" spans="3:5">
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" ht="50" customHeight="1" spans="3:5">
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" ht="50" customHeight="1" spans="3:5">
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" ht="50" customHeight="1" spans="3:5">
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="198" customHeight="1" spans="3:5">
       <c r="C8" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" ht="50" customHeight="1" spans="3:5">
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" ht="50" customHeight="1" spans="3:5">
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" ht="50" customHeight="1" spans="3:5">
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" ht="50" customHeight="1" spans="3:5">
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" ht="50" customHeight="1" spans="3:5">
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" ht="50" customHeight="1" spans="3:5">
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E14" s="5"/>
     </row>

</xml_diff>